<commit_message>
Finished both whisker modules
</commit_message>
<xml_diff>
--- a/Documentation/whisker_system/whisker_module_1_BOM.xlsx
+++ b/Documentation/whisker_system/whisker_module_1_BOM.xlsx
@@ -123,18 +123,9 @@
     <t>Header</t>
   </si>
   <si>
-    <t>3 pin polar</t>
-  </si>
-  <si>
     <t>Molex Inc</t>
   </si>
   <si>
-    <t>WM4201-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/0022232031/WM4201-ND/26669</t>
-  </si>
-  <si>
     <t>5 pin polar</t>
   </si>
   <si>
@@ -178,6 +169,15 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/CD74HCT151E/296-2139-5-ND/38312</t>
+  </si>
+  <si>
+    <t>4 pin polar</t>
+  </si>
+  <si>
+    <t>WM4202-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/dksearch/dksus.dll?vendor=0&amp;keywords=22232041</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,16 +763,16 @@
         <v>27</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I4" s="1">
         <v>0.63</v>
@@ -790,33 +790,33 @@
         <v>34</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="5">
-        <v>22232031</v>
+        <v>22232041</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="I5" s="1">
-        <v>0.3</v>
+        <v>0.37</v>
       </c>
       <c r="J5" s="3">
         <v>1</v>
       </c>
       <c r="K5" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>0.3</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -824,11 +824,11 @@
         <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5">
         <v>22232051</v>
@@ -837,10 +837,10 @@
         <v>22</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I6" s="1">
         <v>0.45</v>
@@ -858,11 +858,11 @@
         <v>34</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="5">
         <v>22232021</v>
@@ -871,10 +871,10 @@
         <v>22</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I7" s="4">
         <v>0.16</v>
@@ -889,26 +889,26 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I8" s="6">
         <v>0.05</v>
@@ -940,7 +940,7 @@
       </c>
       <c r="K10" s="8">
         <f>SUM(Table3[Total])</f>
-        <v>25.29</v>
+        <v>25.36</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1114,30 +1114,29 @@
     <hyperlink ref="G3" r:id="rId6" display="http://www.digikey.com/product-detail/en/SN74LS14NSR/296-3652-1-ND/377690"/>
     <hyperlink ref="D3" r:id="rId7" display="http://digikey.com/Suppliers/us/Texas-Instruments.page?lang=en"/>
     <hyperlink ref="D5" r:id="rId8" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="E5" r:id="rId9" display="http://www.digikey.com/product-detail/en/0022232031/WM4201-ND/26669"/>
-    <hyperlink ref="G5" r:id="rId10" display="http://www.digikey.com/product-detail/en/0022232031/WM4201-ND/26669"/>
-    <hyperlink ref="D6" r:id="rId11" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="E6" r:id="rId12" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
-    <hyperlink ref="G6" r:id="rId13" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
-    <hyperlink ref="H6" r:id="rId14"/>
-    <hyperlink ref="E7" r:id="rId15" display="http://www.digikey.com/product-detail/en/0022232021/WM4200-ND/26667"/>
-    <hyperlink ref="D7" r:id="rId16" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="G7" r:id="rId17" display="http://www.digikey.com/product-detail/en/0022232021/WM4200-ND/26667"/>
-    <hyperlink ref="H8" r:id="rId18"/>
-    <hyperlink ref="G8" r:id="rId19" display="http://www.digikey.com/product-detail/en/CF14JT10K0/CF14JT10K0CT-ND/1830374"/>
-    <hyperlink ref="E8" r:id="rId20" display="http://www.digikey.com/product-detail/en/CF14JT10K0/CF14JT10K0CT-ND/1830374"/>
-    <hyperlink ref="D8" r:id="rId21" display="http://digikey.com/Suppliers/us/Stackpole-Electronics.page?lang=en"/>
-    <hyperlink ref="H3" r:id="rId22"/>
-    <hyperlink ref="D4" r:id="rId23" display="http://digikey.com/Suppliers/us/Texas-Instruments.page?lang=en"/>
-    <hyperlink ref="E4" r:id="rId24" display="http://www.digikey.com/product-detail/en/CD74HCT151E/296-2139-5-ND/38312"/>
-    <hyperlink ref="G4" r:id="rId25" display="http://www.digikey.com/product-detail/en/CD74HCT151E/296-2139-5-ND/38312"/>
-    <hyperlink ref="H5" r:id="rId26"/>
-    <hyperlink ref="H7" r:id="rId27"/>
+    <hyperlink ref="D6" r:id="rId9" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
+    <hyperlink ref="E6" r:id="rId10" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
+    <hyperlink ref="G6" r:id="rId11" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
+    <hyperlink ref="H6" r:id="rId12"/>
+    <hyperlink ref="E7" r:id="rId13" display="http://www.digikey.com/product-detail/en/0022232021/WM4200-ND/26667"/>
+    <hyperlink ref="D7" r:id="rId14" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
+    <hyperlink ref="G7" r:id="rId15" display="http://www.digikey.com/product-detail/en/0022232021/WM4200-ND/26667"/>
+    <hyperlink ref="H8" r:id="rId16"/>
+    <hyperlink ref="G8" r:id="rId17" display="http://www.digikey.com/product-detail/en/CF14JT10K0/CF14JT10K0CT-ND/1830374"/>
+    <hyperlink ref="E8" r:id="rId18" display="http://www.digikey.com/product-detail/en/CF14JT10K0/CF14JT10K0CT-ND/1830374"/>
+    <hyperlink ref="D8" r:id="rId19" display="http://digikey.com/Suppliers/us/Stackpole-Electronics.page?lang=en"/>
+    <hyperlink ref="H3" r:id="rId20"/>
+    <hyperlink ref="D4" r:id="rId21" display="http://digikey.com/Suppliers/us/Texas-Instruments.page?lang=en"/>
+    <hyperlink ref="E4" r:id="rId22" display="http://www.digikey.com/product-detail/en/CD74HCT151E/296-2139-5-ND/38312"/>
+    <hyperlink ref="G4" r:id="rId23" display="http://www.digikey.com/product-detail/en/CD74HCT151E/296-2139-5-ND/38312"/>
+    <hyperlink ref="H7" r:id="rId24"/>
+    <hyperlink ref="G5" r:id="rId25"/>
+    <hyperlink ref="E5" r:id="rId26" display="http://www.digikey.com/scripts/dksearch/dksus.dll?vendor=0&amp;keywords=22232041"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="50" orientation="landscape" r:id="rId28"/>
+  <pageSetup scale="50" orientation="landscape" r:id="rId27"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>